<commit_message>
Light and RailPoint implemented
</commit_message>
<xml_diff>
--- a/station_in_config/Light.xlsx
+++ b/station_in_config/Light.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="570" windowWidth="16425" windowHeight="8385"/>
+    <workbookView xWindow="1920" yWindow="225" windowWidth="16425" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -189,12 +189,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -515,7 +514,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -560,7 +559,7 @@
       <c r="D2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>39</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -677,7 +676,7 @@
       <c r="C8" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="24" t="s">
         <v>34</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -694,10 +693,10 @@
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>37</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -714,10 +713,10 @@
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="20" t="s">
         <v>37</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -734,10 +733,10 @@
       <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="22" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -754,10 +753,10 @@
       <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="24" t="s">
         <v>32</v>
       </c>
       <c r="E12" s="4" t="s">

</xml_diff>